<commit_message>
rm  print array and sheet; add test data in record.xlxs
</commit_message>
<xml_diff>
--- a/record.xlsx
+++ b/record.xlsx
@@ -1,74 +1,75 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+  <si>
+    <t>日期</t>
+  </si>
   <si>
     <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Jerry</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>抓偷奶酪的Tom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>胡蒙</t>
+  </si>
+  <si>
+    <t xml:space="preserve">测试 </t>
+  </si>
+  <si>
+    <t>郭闻浩</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,30 +85,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -407,34 +399,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="8.88671875"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="9.5546875"/>
+    <col customWidth="1" max="16384" min="3" style="1" width="8.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="B2" s="1" t="n">
         <v>20170521</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="C2" t="n">
+        <v>20170522</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="27.6" r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -442,9 +441,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>